<commit_message>
Signed-off-by: yasumasakataoka Signed-off-by: yasumasakataoka
</commit_message>
<xml_diff>
--- a/v084/vendor/引当方式.xlsx
+++ b/v084/vendor/引当方式.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="19395" windowHeight="6705" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="19395" windowHeight="6705" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="49">
   <si>
     <t>TABLE：</t>
     <phoneticPr fontId="1"/>
@@ -247,12 +247,20 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t xml:space="preserve">proc_update_gantt_alloc_fm_trn trn,allocs,trngantt_id　=nil
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>proc_create_self_gantt(trn)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +275,12 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -440,7 +454,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -502,6 +516,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4676,6 +4696,317 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400"/>
             <a:t>発注をかけると</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371599" y="685799"/>
+          <a:ext cx="4791075" cy="1304925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>オーダ作成</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>proc_update_gantt_alloc_fm_trn trn,allocs,trngantt_id</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>=nil</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>trn:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>オーダ</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>   allocs:xxxschs</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>alloctbls</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>情報</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>11765</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>670672</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1383365" y="2847974"/>
+          <a:ext cx="4773707" cy="962025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>オーダ自身の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>trngantts</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>作成　</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>proc_create_self_gantt(trn)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4989,8 +5320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:AY109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AA34" sqref="AA34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6948,13 +7279,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B16:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B16" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="B24" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>